<commit_message>
Se completa la planilla de métricas. Reporte de Code Analyzer
</commit_message>
<xml_diff>
--- a/Documentación/Planilla de Métricas V2.1.xlsx
+++ b/Documentación/Planilla de Métricas V2.1.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="39">
   <si>
     <t>Preparación de la Prueba</t>
   </si>
@@ -119,6 +119,18 @@
   </si>
   <si>
     <t>DESCUBRIENDO NOMBRES REPETIDOS</t>
+  </si>
+  <si>
+    <t>OIA</t>
+  </si>
+  <si>
+    <t>Main</t>
+  </si>
+  <si>
+    <t>NombresRepetidos</t>
+  </si>
+  <si>
+    <t>TestNombresRepetidos</t>
   </si>
 </sst>
 </file>
@@ -824,8 +836,23 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -836,44 +863,23 @@
     <xf numFmtId="0" fontId="1" fillId="8" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="5" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
@@ -883,35 +889,14 @@
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="1" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
@@ -920,6 +905,33 @@
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="2" fillId="7" borderId="4" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="26" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="7" borderId="18" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -979,8 +991,8 @@
           <c:yMode val="edge"/>
           <c:x val="3.3565974707706982E-2"/>
           <c:y val="7.4074152627750078E-2"/>
-          <c:w val="0.40158680164979405"/>
-          <c:h val="0.85185169474450029"/>
+          <c:w val="0.40158680164979416"/>
+          <c:h val="0.85185169474450051"/>
         </c:manualLayout>
       </c:layout>
       <c:pieChart>
@@ -1078,13 +1090,13 @@
                   <c:v>7.6388888888888618E-3</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0</c:v>
+                  <c:v>6.9444444444444198E-3</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0</c:v>
+                  <c:v>1.3888888888888889E-3</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0</c:v>
+                  <c:v>4.097222222222241E-2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1101,7 +1113,7 @@
           <c:yMode val="edge"/>
           <c:x val="0.45060916249105226"/>
           <c:y val="0.22139263648838675"/>
-          <c:w val="0.50307062753519494"/>
+          <c:w val="0.50307062753519505"/>
           <c:h val="0.52354412740966338"/>
         </c:manualLayout>
       </c:layout>
@@ -1126,7 +1138,7 @@
   </c:spPr>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
+    <c:pageMargins b="0.75000000000000044" l="0.7000000000000004" r="0.7000000000000004" t="0.75000000000000044" header="0.30000000000000021" footer="0.30000000000000021"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1454,8 +1466,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:P68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13:N13"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="M22" sqref="M22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="0" defaultRowHeight="15" zeroHeight="1"/>
@@ -1470,10 +1482,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:16" s="10" customFormat="1" ht="23.25" customHeight="1">
-      <c r="B1" s="61" t="s">
+      <c r="B1" s="92" t="s">
         <v>19</v>
       </c>
-      <c r="C1" s="61"/>
+      <c r="C1" s="92"/>
       <c r="D1" s="93" t="s">
         <v>34</v>
       </c>
@@ -1505,12 +1517,12 @@
     </row>
     <row r="3" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A3" s="11"/>
-      <c r="B3" s="62" t="s">
+      <c r="B3" s="67" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="64"/>
+      <c r="C3" s="68"/>
+      <c r="D3" s="68"/>
+      <c r="E3" s="69"/>
       <c r="F3" s="12"/>
       <c r="G3" s="12"/>
       <c r="H3" s="12"/>
@@ -1595,12 +1607,12 @@
     </row>
     <row r="7" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A7" s="11"/>
-      <c r="B7" s="62" t="s">
+      <c r="B7" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="63"/>
-      <c r="E7" s="64"/>
+      <c r="C7" s="68"/>
+      <c r="D7" s="68"/>
+      <c r="E7" s="69"/>
       <c r="F7" s="12"/>
       <c r="G7" s="12"/>
       <c r="H7" s="12"/>
@@ -1685,12 +1697,12 @@
     </row>
     <row r="11" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A11" s="11"/>
-      <c r="B11" s="62" t="s">
+      <c r="B11" s="67" t="s">
         <v>30</v>
       </c>
-      <c r="C11" s="63"/>
-      <c r="D11" s="63"/>
-      <c r="E11" s="64"/>
+      <c r="C11" s="68"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="69"/>
       <c r="F11" s="12"/>
       <c r="G11" s="12"/>
       <c r="H11" s="12"/>
@@ -1775,50 +1787,50 @@
     </row>
     <row r="15" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A15" s="11"/>
-      <c r="B15" s="62" t="s">
+      <c r="B15" s="67" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="63"/>
-      <c r="D15" s="63"/>
-      <c r="E15" s="63"/>
-      <c r="F15" s="63"/>
-      <c r="G15" s="63"/>
-      <c r="H15" s="63"/>
-      <c r="I15" s="63"/>
-      <c r="J15" s="63"/>
-      <c r="K15" s="63"/>
-      <c r="L15" s="63"/>
-      <c r="M15" s="63"/>
-      <c r="N15" s="64"/>
+      <c r="C15" s="68"/>
+      <c r="D15" s="68"/>
+      <c r="E15" s="68"/>
+      <c r="F15" s="68"/>
+      <c r="G15" s="68"/>
+      <c r="H15" s="68"/>
+      <c r="I15" s="68"/>
+      <c r="J15" s="68"/>
+      <c r="K15" s="68"/>
+      <c r="L15" s="68"/>
+      <c r="M15" s="68"/>
+      <c r="N15" s="69"/>
       <c r="O15" s="11"/>
     </row>
     <row r="16" spans="1:16" s="15" customFormat="1" ht="16.5" customHeight="1">
       <c r="A16" s="14"/>
-      <c r="B16" s="74" t="s">
+      <c r="B16" s="88" t="s">
         <v>8</v>
       </c>
-      <c r="C16" s="85" t="s">
+      <c r="C16" s="74" t="s">
         <v>9</v>
       </c>
-      <c r="D16" s="85"/>
-      <c r="E16" s="86"/>
-      <c r="F16" s="87" t="s">
+      <c r="D16" s="74"/>
+      <c r="E16" s="75"/>
+      <c r="F16" s="61" t="s">
         <v>11</v>
       </c>
-      <c r="G16" s="88"/>
-      <c r="H16" s="84" t="s">
+      <c r="G16" s="62"/>
+      <c r="H16" s="63" t="s">
         <v>13</v>
       </c>
-      <c r="I16" s="85"/>
-      <c r="J16" s="86"/>
-      <c r="K16" s="87" t="s">
+      <c r="I16" s="74"/>
+      <c r="J16" s="75"/>
+      <c r="K16" s="61" t="s">
         <v>15</v>
       </c>
-      <c r="L16" s="88"/>
-      <c r="M16" s="84" t="s">
+      <c r="L16" s="62"/>
+      <c r="M16" s="63" t="s">
         <v>17</v>
       </c>
-      <c r="N16" s="89" t="s">
+      <c r="N16" s="64" t="s">
         <v>2</v>
       </c>
       <c r="O16" s="14"/>
@@ -1826,10 +1838,10 @@
     </row>
     <row r="17" spans="1:16" s="15" customFormat="1" ht="30">
       <c r="A17" s="14"/>
-      <c r="B17" s="74"/>
-      <c r="C17" s="85"/>
-      <c r="D17" s="85"/>
-      <c r="E17" s="86"/>
+      <c r="B17" s="88"/>
+      <c r="C17" s="74"/>
+      <c r="D17" s="74"/>
+      <c r="E17" s="75"/>
       <c r="F17" s="39" t="s">
         <v>12</v>
       </c>
@@ -1851,8 +1863,8 @@
       <c r="L17" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="M17" s="84"/>
-      <c r="N17" s="89"/>
+      <c r="M17" s="63"/>
+      <c r="N17" s="64"/>
       <c r="O17" s="14"/>
       <c r="P17" s="18"/>
     </row>
@@ -1862,23 +1874,39 @@
         <f>ROW($B18)-16</f>
         <v>2</v>
       </c>
-      <c r="C18" s="78"/>
-      <c r="D18" s="78"/>
-      <c r="E18" s="79"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="4"/>
-      <c r="H18" s="5"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="53" t="str">
+      <c r="C18" s="76" t="s">
+        <v>35</v>
+      </c>
+      <c r="D18" s="76"/>
+      <c r="E18" s="77"/>
+      <c r="F18" s="3">
+        <v>10</v>
+      </c>
+      <c r="G18" s="4">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="H18" s="5">
+        <v>0.54166666666666663</v>
+      </c>
+      <c r="I18" s="6">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="J18" s="53">
         <f>IFERROR(IF(OR(ISBLANK(H18),ISBLANK(I18)),"",IF(I18&gt;=H18,I18-H18,"Error")),"Error")</f>
-        <v/>
-      </c>
-      <c r="K18" s="7"/>
-      <c r="L18" s="8"/>
-      <c r="M18" s="9"/>
-      <c r="N18" s="54" t="str">
+        <v>6.94444444444553E-4</v>
+      </c>
+      <c r="K18" s="7">
+        <v>0</v>
+      </c>
+      <c r="L18" s="8">
+        <v>0</v>
+      </c>
+      <c r="M18" s="9">
+        <v>12</v>
+      </c>
+      <c r="N18" s="54">
         <f>IFERROR(IF(OR(J18="",ISBLANK(L18)),"",J18+L18),"Error")</f>
-        <v/>
+        <v>6.94444444444553E-4</v>
       </c>
       <c r="O18" s="19"/>
       <c r="P18" s="22"/>
@@ -1889,23 +1917,39 @@
         <f t="shared" ref="B19:B25" si="0">ROW($B19)-16</f>
         <v>3</v>
       </c>
-      <c r="C19" s="78"/>
-      <c r="D19" s="78"/>
-      <c r="E19" s="79"/>
-      <c r="F19" s="3"/>
-      <c r="G19" s="4"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="53" t="str">
+      <c r="C19" s="76" t="s">
+        <v>36</v>
+      </c>
+      <c r="D19" s="76"/>
+      <c r="E19" s="77"/>
+      <c r="F19" s="3">
+        <v>20</v>
+      </c>
+      <c r="G19" s="4">
+        <v>3.472222222222222E-3</v>
+      </c>
+      <c r="H19" s="5">
+        <v>0.54236111111111118</v>
+      </c>
+      <c r="I19" s="6">
+        <v>0.54791666666666672</v>
+      </c>
+      <c r="J19" s="53">
         <f t="shared" ref="J19:J23" si="1">IFERROR(IF(OR(ISBLANK(H19),ISBLANK(I19)),"",IF(I19&gt;=H19,I19-H19,"Error")),"Error")</f>
-        <v/>
-      </c>
-      <c r="K19" s="7"/>
-      <c r="L19" s="8"/>
-      <c r="M19" s="9"/>
-      <c r="N19" s="54" t="str">
+        <v>5.5555555555555358E-3</v>
+      </c>
+      <c r="K19" s="7">
+        <v>0</v>
+      </c>
+      <c r="L19" s="8">
+        <v>0</v>
+      </c>
+      <c r="M19" s="9">
+        <v>40</v>
+      </c>
+      <c r="N19" s="54">
         <f t="shared" ref="N19:N25" si="2">IFERROR(IF(OR(J19="",ISBLANK(L19)),"",J19+L19),"Error")</f>
-        <v/>
+        <v>5.5555555555555358E-3</v>
       </c>
       <c r="O19" s="19"/>
       <c r="P19" s="22"/>
@@ -1916,23 +1960,39 @@
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="C20" s="78"/>
-      <c r="D20" s="78"/>
-      <c r="E20" s="79"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="4"/>
-      <c r="H20" s="5"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="53" t="str">
+      <c r="C20" s="76" t="s">
+        <v>37</v>
+      </c>
+      <c r="D20" s="76"/>
+      <c r="E20" s="77"/>
+      <c r="F20" s="3">
+        <v>80</v>
+      </c>
+      <c r="G20" s="4">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="H20" s="5">
+        <v>0.54861111111111105</v>
+      </c>
+      <c r="I20" s="6">
+        <v>0.57986111111111105</v>
+      </c>
+      <c r="J20" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K20" s="7"/>
-      <c r="L20" s="8"/>
-      <c r="M20" s="9"/>
-      <c r="N20" s="54" t="str">
+        <v>3.125E-2</v>
+      </c>
+      <c r="K20" s="7">
+        <v>1</v>
+      </c>
+      <c r="L20" s="8">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="M20" s="9">
+        <v>61</v>
+      </c>
+      <c r="N20" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>3.2638888888888891E-2</v>
       </c>
       <c r="O20" s="19"/>
       <c r="P20" s="22"/>
@@ -1943,23 +2003,39 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="C21" s="78"/>
-      <c r="D21" s="78"/>
-      <c r="E21" s="79"/>
-      <c r="F21" s="3"/>
-      <c r="G21" s="4"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="6"/>
-      <c r="J21" s="53" t="str">
+      <c r="C21" s="76" t="s">
+        <v>38</v>
+      </c>
+      <c r="D21" s="76"/>
+      <c r="E21" s="77"/>
+      <c r="F21" s="3">
+        <v>60</v>
+      </c>
+      <c r="G21" s="4">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="H21" s="5">
+        <v>0.60416666666666663</v>
+      </c>
+      <c r="I21" s="6">
+        <v>0.60763888888888895</v>
+      </c>
+      <c r="J21" s="53">
         <f t="shared" si="1"/>
-        <v/>
-      </c>
-      <c r="K21" s="7"/>
-      <c r="L21" s="8"/>
-      <c r="M21" s="9"/>
-      <c r="N21" s="54" t="str">
+        <v>3.4722222222223209E-3</v>
+      </c>
+      <c r="K21" s="7">
+        <v>0</v>
+      </c>
+      <c r="L21" s="8">
+        <v>0</v>
+      </c>
+      <c r="M21" s="9">
+        <v>57</v>
+      </c>
+      <c r="N21" s="54">
         <f t="shared" si="2"/>
-        <v/>
+        <v>3.4722222222223209E-3</v>
       </c>
       <c r="O21" s="19"/>
       <c r="P21" s="22"/>
@@ -1970,9 +2046,9 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="C22" s="78"/>
-      <c r="D22" s="78"/>
-      <c r="E22" s="79"/>
+      <c r="C22" s="76"/>
+      <c r="D22" s="76"/>
+      <c r="E22" s="77"/>
       <c r="F22" s="3"/>
       <c r="G22" s="4"/>
       <c r="H22" s="5"/>
@@ -1997,9 +2073,9 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="C23" s="78"/>
-      <c r="D23" s="78"/>
-      <c r="E23" s="79"/>
+      <c r="C23" s="76"/>
+      <c r="D23" s="76"/>
+      <c r="E23" s="77"/>
       <c r="F23" s="3"/>
       <c r="G23" s="4"/>
       <c r="H23" s="5"/>
@@ -2024,9 +2100,9 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="C24" s="78"/>
-      <c r="D24" s="78"/>
-      <c r="E24" s="79"/>
+      <c r="C24" s="76"/>
+      <c r="D24" s="76"/>
+      <c r="E24" s="77"/>
       <c r="F24" s="3"/>
       <c r="G24" s="4"/>
       <c r="H24" s="5"/>
@@ -2045,9 +2121,9 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="C25" s="78"/>
-      <c r="D25" s="78"/>
-      <c r="E25" s="79"/>
+      <c r="C25" s="76"/>
+      <c r="D25" s="76"/>
+      <c r="E25" s="77"/>
       <c r="F25" s="3"/>
       <c r="G25" s="4"/>
       <c r="H25" s="5"/>
@@ -2068,19 +2144,19 @@
     </row>
     <row r="26" spans="1:16" s="27" customFormat="1" ht="15.75" thickBot="1">
       <c r="A26" s="14"/>
-      <c r="B26" s="90" t="s">
+      <c r="B26" s="81" t="s">
         <v>33</v>
       </c>
-      <c r="C26" s="91"/>
-      <c r="D26" s="91"/>
-      <c r="E26" s="92"/>
-      <c r="F26" s="45" t="str">
+      <c r="C26" s="82"/>
+      <c r="D26" s="82"/>
+      <c r="E26" s="83"/>
+      <c r="F26" s="45">
         <f>IF(SUM(F18:F25)=0,"Completar",SUM(F18:F25))</f>
-        <v>Completar</v>
-      </c>
-      <c r="G26" s="46" t="str">
+        <v>170</v>
+      </c>
+      <c r="G26" s="46">
         <f>IF(SUM(G18:G25)=0,"Completar",SUM(G18:G25))</f>
-        <v>Completar</v>
+        <v>3.2638888888888884E-2</v>
       </c>
       <c r="H26" s="47" t="s">
         <v>32</v>
@@ -2088,25 +2164,25 @@
       <c r="I26" s="48" t="s">
         <v>32</v>
       </c>
-      <c r="J26" s="49" t="str">
+      <c r="J26" s="49">
         <f>IF(OR(COUNTIF(J18:J25,"Error")&gt;0,COUNTIF(J18:J25,"Completar")&gt;0),"Error",IF(SUM(J18:J25)=0,"Completar",SUM(J18:J25)))</f>
-        <v>Completar</v>
+        <v>4.097222222222241E-2</v>
       </c>
       <c r="K26" s="50">
         <f>SUM(K18:K25)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L26" s="46">
         <f>SUM(L18:L25)</f>
-        <v>0</v>
-      </c>
-      <c r="M26" s="51" t="str">
+        <v>1.3888888888888889E-3</v>
+      </c>
+      <c r="M26" s="51">
         <f>IF(SUM(M18:M25)=0,"Completar",SUM(M18:M25))</f>
-        <v>Completar</v>
-      </c>
-      <c r="N26" s="52" t="str">
+        <v>170</v>
+      </c>
+      <c r="N26" s="52">
         <f>IF(OR(COUNTIF(N18:N25,"Error")&gt;0,COUNTIF(N18:N25,"Completar")&gt;0),"Error",IF(SUM(N18:N25)=0,"Completar",SUM(N18:N25)))</f>
-        <v>Completar</v>
+        <v>4.2361111111111301E-2</v>
       </c>
       <c r="O26" s="14"/>
       <c r="P26" s="26"/>
@@ -2130,12 +2206,12 @@
     </row>
     <row r="28" spans="1:16" s="13" customFormat="1" ht="15" customHeight="1">
       <c r="A28" s="11"/>
-      <c r="B28" s="62" t="s">
+      <c r="B28" s="67" t="s">
         <v>18</v>
       </c>
-      <c r="C28" s="63"/>
-      <c r="D28" s="63"/>
-      <c r="E28" s="64"/>
+      <c r="C28" s="68"/>
+      <c r="D28" s="68"/>
+      <c r="E28" s="69"/>
       <c r="F28" s="12"/>
       <c r="G28" s="12"/>
       <c r="H28" s="12"/>
@@ -2175,12 +2251,18 @@
     </row>
     <row r="30" spans="1:16" s="23" customFormat="1" ht="15.75" thickBot="1">
       <c r="A30" s="19"/>
-      <c r="B30" s="1"/>
-      <c r="C30" s="2"/>
-      <c r="D30" s="2"/>
-      <c r="E30" s="52" t="str">
+      <c r="B30" s="1">
+        <v>6.9444444444444441E-3</v>
+      </c>
+      <c r="C30" s="2">
+        <v>0.65277777777777779</v>
+      </c>
+      <c r="D30" s="2">
+        <v>0.65972222222222221</v>
+      </c>
+      <c r="E30" s="52">
         <f>IFERROR(IF(OR(ISBLANK(C30),ISBLANK(D30)),"Completar",IF(D30&gt;=C30,D30-C30,"Error")),"Error")</f>
-        <v>Completar</v>
+        <v>6.9444444444444198E-3</v>
       </c>
       <c r="F30" s="19"/>
       <c r="G30" s="19"/>
@@ -2212,33 +2294,33 @@
       <c r="O31" s="21"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="B32" s="62" t="s">
+      <c r="B32" s="67" t="s">
         <v>20</v>
       </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="63"/>
-      <c r="E32" s="63"/>
-      <c r="F32" s="63"/>
-      <c r="G32" s="63"/>
-      <c r="H32" s="63"/>
-      <c r="I32" s="63"/>
-      <c r="J32" s="63"/>
-      <c r="K32" s="63"/>
-      <c r="L32" s="63"/>
-      <c r="M32" s="63"/>
-      <c r="N32" s="64"/>
+      <c r="C32" s="68"/>
+      <c r="D32" s="68"/>
+      <c r="E32" s="68"/>
+      <c r="F32" s="68"/>
+      <c r="G32" s="68"/>
+      <c r="H32" s="68"/>
+      <c r="I32" s="68"/>
+      <c r="J32" s="68"/>
+      <c r="K32" s="68"/>
+      <c r="L32" s="68"/>
+      <c r="M32" s="68"/>
+      <c r="N32" s="69"/>
     </row>
     <row r="33" spans="1:15" ht="15" customHeight="1">
-      <c r="B33" s="69" t="s">
+      <c r="B33" s="78" t="s">
         <v>22</v>
       </c>
-      <c r="C33" s="70"/>
-      <c r="D33" s="71"/>
-      <c r="E33" s="80" t="str">
+      <c r="C33" s="79"/>
+      <c r="D33" s="80"/>
+      <c r="E33" s="72">
         <f>M26</f>
-        <v>Completar</v>
-      </c>
-      <c r="F33" s="81"/>
+        <v>170</v>
+      </c>
+      <c r="F33" s="73"/>
       <c r="G33" s="29"/>
       <c r="H33" s="30"/>
       <c r="I33" s="30"/>
@@ -2249,16 +2331,16 @@
       <c r="N33" s="31"/>
     </row>
     <row r="34" spans="1:15">
-      <c r="B34" s="69" t="s">
+      <c r="B34" s="78" t="s">
         <v>23</v>
       </c>
-      <c r="C34" s="70"/>
-      <c r="D34" s="71"/>
-      <c r="E34" s="82" t="str">
+      <c r="C34" s="79"/>
+      <c r="D34" s="80"/>
+      <c r="E34" s="70">
         <f>IF(M26="Completar","Completar",IFERROR(M26/(N26*24),"Error"))</f>
-        <v>Completar</v>
-      </c>
-      <c r="F34" s="83"/>
+        <v>167.2131147540976</v>
+      </c>
+      <c r="F34" s="71"/>
       <c r="G34" s="32"/>
       <c r="H34" s="33"/>
       <c r="I34" s="33"/>
@@ -2269,16 +2351,16 @@
       <c r="N34" s="34"/>
     </row>
     <row r="35" spans="1:15" ht="15" customHeight="1">
-      <c r="B35" s="69" t="s">
+      <c r="B35" s="78" t="s">
         <v>21</v>
       </c>
-      <c r="C35" s="70"/>
-      <c r="D35" s="71"/>
-      <c r="E35" s="80">
+      <c r="C35" s="79"/>
+      <c r="D35" s="80"/>
+      <c r="E35" s="72">
         <f>IF(K26=0,0,IFERROR(ROUNDUP(K26/(M26/100),0),"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F35" s="81"/>
+        <v>1</v>
+      </c>
+      <c r="F35" s="73"/>
       <c r="G35" s="32"/>
       <c r="H35" s="33"/>
       <c r="I35" s="33"/>
@@ -2289,16 +2371,16 @@
       <c r="N35" s="34"/>
     </row>
     <row r="36" spans="1:15" ht="15" customHeight="1">
-      <c r="B36" s="69" t="s">
+      <c r="B36" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="C36" s="70"/>
-      <c r="D36" s="71"/>
-      <c r="E36" s="67">
+      <c r="C36" s="79"/>
+      <c r="D36" s="80"/>
+      <c r="E36" s="84">
         <f>IF(K26=0,0,IFERROR(K26/M26,"Error"))</f>
-        <v>0</v>
-      </c>
-      <c r="F36" s="68"/>
+        <v>5.8823529411764705E-3</v>
+      </c>
+      <c r="F36" s="85"/>
       <c r="G36" s="32"/>
       <c r="H36" s="33"/>
       <c r="I36" s="33"/>
@@ -2309,18 +2391,18 @@
       <c r="N36" s="34"/>
     </row>
     <row r="37" spans="1:15" ht="15" customHeight="1">
-      <c r="B37" s="69" t="s">
+      <c r="B37" s="78" t="s">
         <v>27</v>
       </c>
-      <c r="C37" s="70"/>
-      <c r="D37" s="71"/>
+      <c r="C37" s="79"/>
+      <c r="D37" s="80"/>
       <c r="E37" s="57">
         <f>E5</f>
         <v>3.4722222222223209E-3</v>
       </c>
       <c r="F37" s="58">
         <f>IF(E37="Completar",E37,IFERROR(E37/$E$43,"Error"))</f>
-        <v>8.0645161290324743E-2</v>
+        <v>3.7593984962406991E-2</v>
       </c>
       <c r="G37" s="32"/>
       <c r="H37" s="33"/>
@@ -2332,18 +2414,18 @@
       <c r="N37" s="34"/>
     </row>
     <row r="38" spans="1:15" ht="15" customHeight="1">
-      <c r="B38" s="69" t="s">
+      <c r="B38" s="78" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="70"/>
-      <c r="D38" s="71"/>
+      <c r="C38" s="79"/>
+      <c r="D38" s="80"/>
       <c r="E38" s="57">
         <f>E9</f>
         <v>3.1944444444444442E-2</v>
       </c>
       <c r="F38" s="58">
         <f>IF(E38="Completar",E38,IFERROR(E38/$E$43,"Error"))</f>
-        <v>0.74193548387096653</v>
+        <v>0.34586466165413449</v>
       </c>
       <c r="G38" s="32"/>
       <c r="H38" s="33"/>
@@ -2355,18 +2437,18 @@
       <c r="N38" s="34"/>
     </row>
     <row r="39" spans="1:15" ht="15" customHeight="1">
-      <c r="B39" s="69" t="s">
+      <c r="B39" s="78" t="s">
         <v>31</v>
       </c>
-      <c r="C39" s="70"/>
-      <c r="D39" s="71"/>
+      <c r="C39" s="79"/>
+      <c r="D39" s="80"/>
       <c r="E39" s="57">
         <f>E13</f>
         <v>7.6388888888888618E-3</v>
       </c>
       <c r="F39" s="58">
         <f t="shared" ref="F39" si="3">IF(E39="Completar",E39,IFERROR(E39/$E$43,"Error"))</f>
-        <v>0.17741935483870877</v>
+        <v>8.2706766917292743E-2</v>
       </c>
       <c r="G39" s="32"/>
       <c r="H39" s="33"/>
@@ -2378,18 +2460,18 @@
       <c r="N39" s="34"/>
     </row>
     <row r="40" spans="1:15" ht="15" customHeight="1">
-      <c r="B40" s="69" t="s">
+      <c r="B40" s="78" t="s">
         <v>29</v>
       </c>
-      <c r="C40" s="70"/>
-      <c r="D40" s="71"/>
-      <c r="E40" s="57" t="str">
+      <c r="C40" s="79"/>
+      <c r="D40" s="80"/>
+      <c r="E40" s="57">
         <f>E30</f>
-        <v>Completar</v>
-      </c>
-      <c r="F40" s="58" t="str">
+        <v>6.9444444444444198E-3</v>
+      </c>
+      <c r="F40" s="58">
         <f>IF(E40="Completar",E40,IFERROR(E40/$E$43,"Error"))</f>
-        <v>Completar</v>
+        <v>7.5187969924811582E-2</v>
       </c>
       <c r="G40" s="32"/>
       <c r="H40" s="33"/>
@@ -2401,18 +2483,18 @@
       <c r="N40" s="34"/>
     </row>
     <row r="41" spans="1:15" ht="15" customHeight="1">
-      <c r="B41" s="69" t="s">
+      <c r="B41" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="C41" s="70"/>
-      <c r="D41" s="71"/>
+      <c r="C41" s="79"/>
+      <c r="D41" s="80"/>
       <c r="E41" s="57">
         <f>L26</f>
-        <v>0</v>
+        <v>1.3888888888888889E-3</v>
       </c>
       <c r="F41" s="58">
         <f>IF(E41="Completar",E41,IFERROR(E41/$E$43,"Completar"))</f>
-        <v>0</v>
+        <v>1.503759398496237E-2</v>
       </c>
       <c r="G41" s="32"/>
       <c r="H41" s="33"/>
@@ -2424,18 +2506,18 @@
       <c r="N41" s="34"/>
     </row>
     <row r="42" spans="1:15" ht="15" customHeight="1">
-      <c r="B42" s="69" t="s">
+      <c r="B42" s="78" t="s">
         <v>26</v>
       </c>
-      <c r="C42" s="70"/>
-      <c r="D42" s="71"/>
-      <c r="E42" s="57" t="str">
+      <c r="C42" s="79"/>
+      <c r="D42" s="80"/>
+      <c r="E42" s="57">
         <f>J26</f>
-        <v>Completar</v>
-      </c>
-      <c r="F42" s="58" t="str">
+        <v>4.097222222222241E-2</v>
+      </c>
+      <c r="F42" s="58">
         <f>IF(E42="Completar",E42,IFERROR(E42/$E$43,"Completar"))</f>
-        <v>Completar</v>
+        <v>0.4436090225563919</v>
       </c>
       <c r="G42" s="32"/>
       <c r="H42" s="33"/>
@@ -2447,16 +2529,16 @@
       <c r="N42" s="34"/>
     </row>
     <row r="43" spans="1:15" ht="15" customHeight="1" thickBot="1">
-      <c r="B43" s="75" t="s">
+      <c r="B43" s="89" t="s">
         <v>6</v>
       </c>
-      <c r="C43" s="76"/>
-      <c r="D43" s="77"/>
-      <c r="E43" s="72">
+      <c r="C43" s="90"/>
+      <c r="D43" s="91"/>
+      <c r="E43" s="86">
         <f>IF(COUNTIF(E37:E42,"Error")&gt;0,"Error",IF(SUM(E37:E42)=0,"Completar",SUM(E37:E42)))</f>
-        <v>4.3055555555555625E-2</v>
-      </c>
-      <c r="F43" s="73"/>
+        <v>9.2361111111111338E-2</v>
+      </c>
+      <c r="F43" s="87"/>
       <c r="G43" s="35"/>
       <c r="H43" s="36"/>
       <c r="I43" s="36"/>
@@ -2497,27 +2579,13 @@
   </sheetData>
   <sheetProtection formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" deleteColumns="0" deleteRows="0"/>
   <mergeCells count="44">
-    <mergeCell ref="K16:L16"/>
-    <mergeCell ref="M16:M17"/>
-    <mergeCell ref="N16:N17"/>
-    <mergeCell ref="F8:N8"/>
-    <mergeCell ref="F9:N9"/>
-    <mergeCell ref="B15:N15"/>
-    <mergeCell ref="E34:F34"/>
-    <mergeCell ref="E35:F35"/>
-    <mergeCell ref="H16:J16"/>
-    <mergeCell ref="F16:G16"/>
-    <mergeCell ref="C16:E17"/>
-    <mergeCell ref="C21:E21"/>
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="C24:E24"/>
-    <mergeCell ref="B28:E28"/>
-    <mergeCell ref="B33:D33"/>
-    <mergeCell ref="C22:E22"/>
-    <mergeCell ref="C23:E23"/>
-    <mergeCell ref="C25:E25"/>
-    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="B1:C1"/>
+    <mergeCell ref="D1:N1"/>
+    <mergeCell ref="B11:E11"/>
+    <mergeCell ref="F12:N12"/>
+    <mergeCell ref="F13:N13"/>
+    <mergeCell ref="B7:E7"/>
+    <mergeCell ref="B3:E3"/>
     <mergeCell ref="E36:F36"/>
     <mergeCell ref="B42:D42"/>
     <mergeCell ref="E43:F43"/>
@@ -2534,13 +2602,27 @@
     <mergeCell ref="C18:E18"/>
     <mergeCell ref="B39:D39"/>
     <mergeCell ref="E33:F33"/>
-    <mergeCell ref="B1:C1"/>
-    <mergeCell ref="D1:N1"/>
-    <mergeCell ref="B11:E11"/>
-    <mergeCell ref="F12:N12"/>
-    <mergeCell ref="F13:N13"/>
-    <mergeCell ref="B7:E7"/>
-    <mergeCell ref="B3:E3"/>
+    <mergeCell ref="E34:F34"/>
+    <mergeCell ref="E35:F35"/>
+    <mergeCell ref="H16:J16"/>
+    <mergeCell ref="F16:G16"/>
+    <mergeCell ref="C16:E17"/>
+    <mergeCell ref="C21:E21"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="C24:E24"/>
+    <mergeCell ref="B28:E28"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="C22:E22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="C25:E25"/>
+    <mergeCell ref="B26:E26"/>
+    <mergeCell ref="K16:L16"/>
+    <mergeCell ref="M16:M17"/>
+    <mergeCell ref="N16:N17"/>
+    <mergeCell ref="F8:N8"/>
+    <mergeCell ref="F9:N9"/>
+    <mergeCell ref="B15:N15"/>
   </mergeCells>
   <conditionalFormatting sqref="A1:B1048576 D1:XFD1048576 C3:C1048576">
     <cfRule type="cellIs" dxfId="1" priority="1" operator="equal">

</xml_diff>